<commit_message>
Write method to compare the different QC criteria and run t-test
About to delete all my notebook code, if everything goes wrong roll back to here!
</commit_message>
<xml_diff>
--- a/02_meter_data/gas_analysis_standards.xlsx
+++ b/02_meter_data/gas_analysis_standards.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13576F2A-ED03-1740-9380-04BC5226FD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734D87E2-CC34-4143-891C-E07C4FF8BB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35020" yWindow="540" windowWidth="37740" windowHeight="19260" activeTab="1" xr2:uid="{E854F3CC-68B1-C643-8758-04060BCC422B}"/>
+    <workbookView xWindow="34620" yWindow="500" windowWidth="15120" windowHeight="19540" activeTab="1" xr2:uid="{E854F3CC-68B1-C643-8758-04060BCC422B}"/>
   </bookViews>
   <sheets>
     <sheet name="Standards" sheetId="1" r:id="rId1"/>
     <sheet name="Samples" sheetId="2" r:id="rId2"/>
     <sheet name="Normalization" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I3:I15" si="0">D6-G6</f>
+        <f t="shared" ref="I6:I15" si="0">D6-G6</f>
         <v>-5.3062517970547951E-5</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1891,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9EA058-2D94-C84E-A5D3-668D2FA9838E}">
   <dimension ref="A1:AE81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>